<commit_message>
Estabilización de Monitor Dual, Instructivo y Scraper Real
</commit_message>
<xml_diff>
--- a/data/reporte_fenomenos_20260129.xlsx
+++ b/data/reporte_fenomenos_20260129.xlsx
@@ -7,7 +7,8 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Analisis" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Glosario" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -425,7 +426,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:L13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -441,12 +442,57 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
+          <t>nro_proceso</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
           <t>detalle</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>estado</t>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>tipo_proceso</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>link</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>fuente</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>texto_clean</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>tipo_decision</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>transferencia</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>indice_total</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>indice_fenomeno_corruptivo</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>nivel_riesgo_teorico</t>
         </is>
       </c>
     </row>
@@ -458,12 +504,758 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Análisis automático de fenómenos corruptivos - BORA</t>
+          <t>ADQUISICION DE ELEMENTOS DE LIBRERIA</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Procesado</t>
+          <t>Licitación Privada</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>30/01/2026 07:00 Hrs.</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>https://comprar.gob.ar/Compras.aspx?qs=W1HXHGHtH10=</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>Scraper Automático Comprar</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>licitacion privada</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>Traslado de Impuestos</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>Contribuyentes al Estado</t>
+        </is>
+      </c>
+      <c r="J2" t="n">
+        <v>9.5</v>
+      </c>
+      <c r="K2" t="n">
+        <v>9.5</v>
+      </c>
+      <c r="L2" t="inlineStr">
+        <is>
+          <t>Alto</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>2026-01-29</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>ADQUISICION DE ELEMENTOS DE BAZAR</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Licitación Privada</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>30/01/2026 07:00 Hrs.</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>https://comprar.gob.ar/Compras.aspx?qs=W1HXHGHtH10=</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>Scraper Automático Comprar</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>licitacion privada</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>Traslado de Impuestos</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>Contribuyentes al Estado</t>
+        </is>
+      </c>
+      <c r="J3" t="n">
+        <v>9.5</v>
+      </c>
+      <c r="K3" t="n">
+        <v>9.5</v>
+      </c>
+      <c r="L3" t="inlineStr">
+        <is>
+          <t>Alto</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>2026-01-29</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>SERVICIO DE TRANSPORTE CHARTER PARA ALUMNOS Y CADETES.</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Licitación Privada</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>30/01/2026 08:00 Hrs.</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>https://comprar.gob.ar/Compras.aspx?qs=W1HXHGHtH10=</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>Scraper Automático Comprar</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>licitacion privada</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>Traslado de Impuestos</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>Contribuyentes al Estado</t>
+        </is>
+      </c>
+      <c r="J4" t="n">
+        <v>9.5</v>
+      </c>
+      <c r="K4" t="n">
+        <v>9.5</v>
+      </c>
+      <c r="L4" t="inlineStr">
+        <is>
+          <t>Alto</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>2026-01-29</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>SERVICIO DE RECARGA DE GAS A GRANEL (ZEPPELIN) PARA EL CDO BR BL II - 1er SEMESTRE 2026</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Licitación Privada</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>30/01/2026 08:00 Hrs.</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>https://comprar.gob.ar/Compras.aspx?qs=W1HXHGHtH10=</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>Scraper Automático Comprar</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>licitacion privada</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>Traslado de Impuestos</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>Contribuyentes al Estado</t>
+        </is>
+      </c>
+      <c r="J5" t="n">
+        <v>9.5</v>
+      </c>
+      <c r="K5" t="n">
+        <v>9.5</v>
+      </c>
+      <c r="L5" t="inlineStr">
+        <is>
+          <t>Alto</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>2026-01-29</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>SERVICIO DE MANTENIMIENTO Y REPARACIÓN DE ASCENSOR</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Contratación Directa</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>30/01/2026 08:00 Hrs.</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>https://comprar.gob.ar/Compras.aspx?qs=W1HXHGHtH10=</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>Scraper Automático Comprar</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>contratacion directa</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>Contratos Públicos</t>
+        </is>
+      </c>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>Estado a Empresas Contratistas</t>
+        </is>
+      </c>
+      <c r="J6" t="n">
+        <v>8.5</v>
+      </c>
+      <c r="K6" t="n">
+        <v>8.5</v>
+      </c>
+      <c r="L6" t="inlineStr">
+        <is>
+          <t>Alto</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>2026-01-29</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Servicio de fumigación para el CGMBA</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>Licitación Privada</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>30/01/2026 08:00 Hrs.</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>https://comprar.gob.ar/Compras.aspx?qs=W1HXHGHtH10=</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>Scraper Automático Comprar</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>licitacion privada</t>
+        </is>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>Traslado de Impuestos</t>
+        </is>
+      </c>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>Contribuyentes al Estado</t>
+        </is>
+      </c>
+      <c r="J7" t="n">
+        <v>9.5</v>
+      </c>
+      <c r="K7" t="n">
+        <v>9.5</v>
+      </c>
+      <c r="L7" t="inlineStr">
+        <is>
+          <t>Alto</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>2026-01-29</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Mantenimiento y reparación de edificios (Rancho de Tropas) del CGMBA</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>Licitación Privada</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>30/01/2026 08:00 Hrs.</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>https://comprar.gob.ar/Compras.aspx?qs=W1HXHGHtH10=</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>Scraper Automático Comprar</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>licitacion privada</t>
+        </is>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>Traslado de Impuestos</t>
+        </is>
+      </c>
+      <c r="I8" t="inlineStr">
+        <is>
+          <t>Contribuyentes al Estado</t>
+        </is>
+      </c>
+      <c r="J8" t="n">
+        <v>9.5</v>
+      </c>
+      <c r="K8" t="n">
+        <v>9.5</v>
+      </c>
+      <c r="L8" t="inlineStr">
+        <is>
+          <t>Alto</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>2026-01-29</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>ALQUILER DE SISTEMA INFORMÁTICO DE LABORATORIO PARA EL HMRP –2026.</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>Licitación Privada</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>30/01/2026 08:00 Hrs.</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>https://comprar.gob.ar/Compras.aspx?qs=W1HXHGHtH10=</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>Scraper Automático Comprar</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>licitacion privada</t>
+        </is>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>Traslado de Impuestos</t>
+        </is>
+      </c>
+      <c r="I9" t="inlineStr">
+        <is>
+          <t>Contribuyentes al Estado</t>
+        </is>
+      </c>
+      <c r="J9" t="n">
+        <v>9.5</v>
+      </c>
+      <c r="K9" t="n">
+        <v>9.5</v>
+      </c>
+      <c r="L9" t="inlineStr">
+        <is>
+          <t>Alto</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>2026-01-29</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>ADQUISICIÓN DE VIVERES ESPECIALES Y HOSPITALARIOS PARA EL CDO BR BL II Y UNIDADES DEPENDIENTES–2026</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>Licitación Privada</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>30/01/2026 08:00 Hrs.</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>https://comprar.gob.ar/Compras.aspx?qs=W1HXHGHtH10=</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>Scraper Automático Comprar</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>licitacion privada</t>
+        </is>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>Traslado de Impuestos</t>
+        </is>
+      </c>
+      <c r="I10" t="inlineStr">
+        <is>
+          <t>Contribuyentes al Estado</t>
+        </is>
+      </c>
+      <c r="J10" t="n">
+        <v>9.5</v>
+      </c>
+      <c r="K10" t="n">
+        <v>9.5</v>
+      </c>
+      <c r="L10" t="inlineStr">
+        <is>
+          <t>Alto</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>2026-01-29</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>Adquisición de víveres especiales para el CGMBA</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>Licitación Privada</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>30/01/2026 08:00 Hrs.</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>https://comprar.gob.ar/Compras.aspx?qs=W1HXHGHtH10=</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>Scraper Automático Comprar</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>licitacion privada</t>
+        </is>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>Traslado de Impuestos</t>
+        </is>
+      </c>
+      <c r="I11" t="inlineStr">
+        <is>
+          <t>Contribuyentes al Estado</t>
+        </is>
+      </c>
+      <c r="J11" t="n">
+        <v>9.5</v>
+      </c>
+      <c r="K11" t="n">
+        <v>9.5</v>
+      </c>
+      <c r="L11" t="inlineStr">
+        <is>
+          <t>Alto</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>2026-01-29</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>https://comprar.gob.arjavascript:__doPostBack('ctl00$CPH1$GridListaPliegosAperturaProxima','Page$2')</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>Scraper Automático Comprar</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>No identificado</t>
+        </is>
+      </c>
+      <c r="I12" t="inlineStr">
+        <is>
+          <t>No identificado</t>
+        </is>
+      </c>
+      <c r="J12" t="n">
+        <v>0</v>
+      </c>
+      <c r="K12" t="n">
+        <v>0</v>
+      </c>
+      <c r="L12" t="inlineStr">
+        <is>
+          <t>Bajo</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>2026-01-29</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>https://comprar.gob.arjavascript:__doPostBack('ctl00$CPH1$GridListaPliegosAperturaProxima','Page$3')</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>Scraper Automático Comprar</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>No identificado</t>
+        </is>
+      </c>
+      <c r="I13" t="inlineStr">
+        <is>
+          <t>No identificado</t>
+        </is>
+      </c>
+      <c r="J13" t="n">
+        <v>0</v>
+      </c>
+      <c r="K13" t="n">
+        <v>0</v>
+      </c>
+      <c r="L13" t="inlineStr">
+        <is>
+          <t>Bajo</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Variable</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Definición</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>tipo_decision</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Escenario detectado de la Gran Corrupción.</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>transferencia</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Sector económico afectado por la medida.</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>indice_fenomeno_corruptivo</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Intensidad del fenómeno (0-10).</t>
         </is>
       </c>
     </row>

</xml_diff>